<commit_message>
Add most recent YPE data from Google Drive
</commit_message>
<xml_diff>
--- a/Data/RawData/YPE_Data/YPE_60_LowerWawonaPoint/Digital Data_YPE60/YPE_Understory_Plot_60.xlsx
+++ b/Data/RawData/YPE_Data/YPE_60_LowerWawonaPoint/Digital Data_YPE60/YPE_Understory_Plot_60.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="nj2GFW4uj6fuD7M1mLtnd685xwW7piKHlG/HSg7if9A="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="pKsft7l5AvSh1aBykvC++m/pjieVGddtPNLYytykDoU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -32,14 +32,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miMjP1VrZdqIPx0HOcATtyMz5yRoA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgF95DKZZaX2OB4txqaOa6F0h056w=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="71">
   <si>
     <t>plotID</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>ABCO_seed</t>
-  </si>
-  <si>
-    <t>DIGL</t>
   </si>
   <si>
     <t>wood</t>
@@ -810,7 +807,7 @@
         <v>40</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S3" s="4" t="s">
         <v>42</v>
@@ -884,7 +881,7 @@
         <v>2.0</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>36</v>
@@ -920,7 +917,7 @@
         <v>40</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S4" s="4" t="s">
         <v>42</v>
@@ -1030,7 +1027,7 @@
         <v>40</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S5" s="4" t="s">
         <v>42</v>
@@ -1140,7 +1137,7 @@
         <v>40</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S6" s="4" t="s">
         <v>42</v>
@@ -1214,7 +1211,7 @@
         <v>5.0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>38</v>
@@ -1250,7 +1247,7 @@
         <v>40</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S7" s="4" t="s">
         <v>42</v>
@@ -1360,7 +1357,7 @@
         <v>40</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S8" s="4" t="s">
         <v>42</v>
@@ -1470,7 +1467,7 @@
         <v>40</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>42</v>
@@ -1580,7 +1577,7 @@
         <v>40</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>42</v>
@@ -1654,7 +1651,7 @@
         <v>9.0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>36</v>
@@ -1690,7 +1687,7 @@
         <v>40</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S11" s="4" t="s">
         <v>42</v>
@@ -1764,7 +1761,7 @@
         <v>10.0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>36</v>
@@ -1800,7 +1797,7 @@
         <v>40</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S12" s="4" t="s">
         <v>42</v>
@@ -1910,7 +1907,7 @@
         <v>40</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S13" s="4" t="s">
         <v>42</v>
@@ -1984,7 +1981,7 @@
         <v>12.0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>36</v>
@@ -2020,7 +2017,7 @@
         <v>40</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S14" s="4" t="s">
         <v>42</v>
@@ -2130,7 +2127,7 @@
         <v>40</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S15" s="4" t="s">
         <v>42</v>
@@ -2204,7 +2201,7 @@
         <v>14.0</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>36</v>
@@ -2240,7 +2237,7 @@
         <v>40</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S16" s="4" t="s">
         <v>42</v>
@@ -2350,7 +2347,7 @@
         <v>40</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S17" s="4" t="s">
         <v>42</v>
@@ -2460,7 +2457,7 @@
         <v>40</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S18" s="4" t="s">
         <v>42</v>
@@ -2534,7 +2531,7 @@
         <v>17.0</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>36</v>
@@ -2570,7 +2567,7 @@
         <v>40</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S19" s="4" t="s">
         <v>42</v>
@@ -2680,7 +2677,7 @@
         <v>40</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S20" s="4" t="s">
         <v>42</v>
@@ -2790,7 +2787,7 @@
         <v>40</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S21" s="4" t="s">
         <v>42</v>
@@ -2864,7 +2861,7 @@
         <v>20.0</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>36</v>
@@ -2900,7 +2897,7 @@
         <v>40</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S22" s="4" t="s">
         <v>42</v>
@@ -3010,7 +3007,7 @@
         <v>40</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S23" s="4" t="s">
         <v>42</v>
@@ -3084,7 +3081,7 @@
         <v>22.0</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>36</v>
@@ -3120,7 +3117,7 @@
         <v>40</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S24" s="4" t="s">
         <v>42</v>
@@ -3194,7 +3191,7 @@
         <v>23.0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>36</v>
@@ -3230,7 +3227,7 @@
         <v>40</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S25" s="4" t="s">
         <v>42</v>
@@ -3340,7 +3337,7 @@
         <v>40</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S26" s="4" t="s">
         <v>42</v>
@@ -3450,7 +3447,7 @@
         <v>40</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S27" s="4" t="s">
         <v>42</v>
@@ -3524,7 +3521,7 @@
         <v>26.0</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>38</v>
@@ -3560,7 +3557,7 @@
         <v>40</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S28" s="4" t="s">
         <v>42</v>
@@ -3670,7 +3667,7 @@
         <v>40</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S29" s="4" t="s">
         <v>42</v>
@@ -3744,7 +3741,7 @@
         <v>28.0</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>38</v>
@@ -3780,7 +3777,7 @@
         <v>40</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S30" s="4" t="s">
         <v>42</v>
@@ -3890,7 +3887,7 @@
         <v>40</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S31" s="4" t="s">
         <v>42</v>
@@ -4000,7 +3997,7 @@
         <v>40</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S32" s="4" t="s">
         <v>42</v>
@@ -4110,7 +4107,7 @@
         <v>40</v>
       </c>
       <c r="R33" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S33" s="4" t="s">
         <v>42</v>
@@ -4220,7 +4217,7 @@
         <v>40</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S34" s="4" t="s">
         <v>42</v>
@@ -4294,13 +4291,13 @@
         <v>33.0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H35" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>36</v>
@@ -4330,7 +4327,7 @@
         <v>40</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S35" s="4" t="s">
         <v>42</v>
@@ -4404,19 +4401,19 @@
         <v>34.0</v>
       </c>
       <c r="F36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="J36" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>38</v>
@@ -4440,7 +4437,7 @@
         <v>40</v>
       </c>
       <c r="R36" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S36" s="4" t="s">
         <v>42</v>
@@ -4514,7 +4511,7 @@
         <v>35.0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G37" s="4" t="s">
         <v>38</v>
@@ -4550,7 +4547,7 @@
         <v>40</v>
       </c>
       <c r="R37" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S37" s="4" t="s">
         <v>42</v>
@@ -4660,7 +4657,7 @@
         <v>40</v>
       </c>
       <c r="R38" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S38" s="4" t="s">
         <v>42</v>
@@ -4734,7 +4731,7 @@
         <v>37.0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G39" s="4" t="s">
         <v>36</v>
@@ -4770,7 +4767,7 @@
         <v>40</v>
       </c>
       <c r="R39" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S39" s="4" t="s">
         <v>42</v>
@@ -4880,7 +4877,7 @@
         <v>40</v>
       </c>
       <c r="R40" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S40" s="4" t="s">
         <v>42</v>
@@ -4957,7 +4954,7 @@
         <v>38</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>36</v>
@@ -4990,7 +4987,7 @@
         <v>40</v>
       </c>
       <c r="R41" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S41" s="4" t="s">
         <v>42</v>
@@ -5064,10 +5061,10 @@
         <v>40.0</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>38</v>
@@ -5100,7 +5097,7 @@
         <v>40</v>
       </c>
       <c r="R42" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S42" s="4" t="s">
         <v>42</v>
@@ -5174,7 +5171,7 @@
         <v>41.0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>36</v>
@@ -5210,7 +5207,7 @@
         <v>40</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S43" s="4" t="s">
         <v>42</v>
@@ -5284,7 +5281,7 @@
         <v>42.0</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>38</v>
@@ -5320,7 +5317,7 @@
         <v>40</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S44" s="4" t="s">
         <v>42</v>
@@ -5394,7 +5391,7 @@
         <v>43.0</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G45" s="4" t="s">
         <v>38</v>
@@ -5430,7 +5427,7 @@
         <v>40</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S45" s="4" t="s">
         <v>42</v>
@@ -5540,7 +5537,7 @@
         <v>40</v>
       </c>
       <c r="R46" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S46" s="4" t="s">
         <v>42</v>
@@ -5650,7 +5647,7 @@
         <v>40</v>
       </c>
       <c r="R47" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S47" s="4" t="s">
         <v>42</v>
@@ -5724,7 +5721,7 @@
         <v>46.0</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G48" s="4" t="s">
         <v>38</v>
@@ -5760,7 +5757,7 @@
         <v>40</v>
       </c>
       <c r="R48" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S48" s="4" t="s">
         <v>42</v>
@@ -5870,7 +5867,7 @@
         <v>40</v>
       </c>
       <c r="R49" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S49" s="4" t="s">
         <v>42</v>
@@ -5980,7 +5977,7 @@
         <v>40</v>
       </c>
       <c r="R50" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S50" s="4" t="s">
         <v>42</v>
@@ -6054,7 +6051,7 @@
         <v>49.0</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G51" s="4" t="s">
         <v>38</v>
@@ -6090,7 +6087,7 @@
         <v>40</v>
       </c>
       <c r="R51" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S51" s="4" t="s">
         <v>42</v>
@@ -6200,7 +6197,7 @@
         <v>40</v>
       </c>
       <c r="R52" s="4" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="S52" s="4" t="s">
         <v>42</v>

</xml_diff>